<commit_message>
change in high level estimation
</commit_message>
<xml_diff>
--- a/ScenarioTwo/IdentityPOC_ScenarioTwo.xlsx
+++ b/ScenarioTwo/IdentityPOC_ScenarioTwo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Not Started</t>
-  </si>
-  <si>
-    <t>Implement logic for user authentication in web app II</t>
   </si>
   <si>
     <t>Active</t>
@@ -135,11 +132,14 @@
   <si>
     <t>IdentityPOC_ScenarioTwo</t>
   </si>
+  <si>
+    <t>Implement logic for user authentication in web app I &amp; II</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,29 +493,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Closed" xfId="2"/>
+    <cellStyle name="Closed" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Not Started" xfId="1"/>
+    <cellStyle name="Not Started" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -713,14 +713,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table5" displayName="Table5" ref="E5:I27" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="E5:I27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="E5:I27" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="E5:I27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="User Story" dataDxfId="4"/>
-    <tableColumn id="2" name="Tasks" dataDxfId="3"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="2"/>
-    <tableColumn id="3" name="Status" dataDxfId="1"/>
-    <tableColumn id="4" name="# Days" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="User Story" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tasks" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned To" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="# Days" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1022,11 +1022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,22 +1039,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E2" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="56"/>
+      <c r="E2" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E3" s="48"/>
-      <c r="F3" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
+      <c r="F3" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D4" s="11"/>
@@ -1062,7 +1062,7 @@
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>22</v>
@@ -1119,10 +1119,10 @@
         <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="42"/>
       <c r="J8" s="11"/>
@@ -1134,10 +1134,10 @@
         <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="42"/>
       <c r="J9" s="11"/>
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>22</v>
@@ -1164,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>22</v>
@@ -1201,10 +1201,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="45"/>
       <c r="J14" s="11"/>
@@ -1216,10 +1216,10 @@
         <v>18</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" s="45"/>
       <c r="J15" s="11"/>
@@ -1228,10 +1228,10 @@
       <c r="D16" s="11"/>
       <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" s="30" t="s">
         <v>22</v>
@@ -1257,7 +1257,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" s="11"/>
     </row>
@@ -1268,7 +1268,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>22</v>
@@ -1283,7 +1283,7 @@
         <v>14</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="30" t="s">
         <v>22</v>
@@ -1298,7 +1298,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="30" t="s">
         <v>22</v>
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="30" t="s">
         <v>22</v>
@@ -1350,7 +1350,7 @@
         <v>19</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="30" t="s">
         <v>22</v>
@@ -1365,7 +1365,7 @@
         <v>20</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H26" s="30" t="s">
         <v>22</v>
@@ -1397,13 +1397,13 @@
     <mergeCell ref="F3:H3"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$S$6:$S$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Not Started, Active, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Aniket, Mrunal, Mahuya"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>